<commit_message>
Merge a requerimientos no funcionales
</commit_message>
<xml_diff>
--- a/riesgos.xlsx
+++ b/riesgos.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Impactos" sheetId="1" r:id="rId1"/>
@@ -345,8 +345,6 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
@@ -355,57 +353,13 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="21">
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color auto="1"/>
-        <name val="Raleway"/>
-        <scheme val="none"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color auto="1"/>
-        <name val="Raleway"/>
-        <scheme val="none"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -524,11 +478,17 @@
     </dxf>
     <dxf>
       <font>
+        <b val="0"/>
+        <i val="0"/>
         <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
         <outline val="0"/>
         <shadow val="0"/>
         <u val="none"/>
         <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
         <name val="Raleway"/>
         <scheme val="none"/>
       </font>
@@ -537,6 +497,7 @@
           <bgColor auto="1"/>
         </patternFill>
       </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -551,6 +512,150 @@
         <vertAlign val="baseline"/>
         <sz val="11"/>
         <color auto="1"/>
+        <name val="Raleway"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Raleway"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor rgb="FFD9D9D9"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Raleway"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="13" formatCode="0%"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor rgb="FFD9D9D9"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Raleway"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor rgb="FFD9D9D9"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Raleway"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor rgb="FFD9D9D9"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Raleway"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor rgb="FFD9D9D9"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
         <name val="Raleway"/>
         <scheme val="none"/>
       </font>
@@ -667,41 +772,11 @@
     </dxf>
     <dxf>
       <font>
-        <b val="0"/>
-        <i val="0"/>
         <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
         <outline val="0"/>
         <shadow val="0"/>
         <u val="none"/>
         <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color auto="1"/>
-        <name val="Raleway"/>
-        <scheme val="none"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor rgb="FFD9D9D9"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
         <name val="Raleway"/>
         <scheme val="none"/>
       </font>
@@ -710,7 +785,6 @@
           <bgColor auto="1"/>
         </patternFill>
       </fill>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -730,80 +804,6 @@
       </font>
       <fill>
         <patternFill patternType="none">
-          <fgColor rgb="FFD9D9D9"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color auto="1"/>
-        <name val="Raleway"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="13" formatCode="0%"/>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor rgb="FFD9D9D9"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color auto="1"/>
-        <name val="Raleway"/>
-        <scheme val="none"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor rgb="FFD9D9D9"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color auto="1"/>
-        <name val="Raleway"/>
-        <scheme val="none"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor rgb="FFD9D9D9"/>
           <bgColor auto="1"/>
         </patternFill>
       </fill>
@@ -823,45 +823,45 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabla1" displayName="Tabla1" ref="A1:F18" totalsRowShown="0" headerRowDxfId="8" dataDxfId="7">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabla1" displayName="Tabla1" ref="A1:F18" totalsRowShown="0" headerRowDxfId="20" dataDxfId="19">
   <autoFilter ref="A1:F18"/>
   <tableColumns count="6">
-    <tableColumn id="1" name="Objetivos del proyecto" dataDxfId="14"/>
-    <tableColumn id="2" name="Muy bajo .05" dataDxfId="13"/>
-    <tableColumn id="3" name="Bajo .1" dataDxfId="12"/>
-    <tableColumn id="4" name="Moderado .2" dataDxfId="11"/>
-    <tableColumn id="5" name="Alto .4" dataDxfId="10"/>
-    <tableColumn id="6" name="Muy alto .8" dataDxfId="9"/>
+    <tableColumn id="1" name="Objetivos del proyecto" dataDxfId="18"/>
+    <tableColumn id="2" name="Muy bajo .05" dataDxfId="17"/>
+    <tableColumn id="3" name="Bajo .1" dataDxfId="16"/>
+    <tableColumn id="4" name="Moderado .2" dataDxfId="15"/>
+    <tableColumn id="5" name="Alto .4" dataDxfId="14"/>
+    <tableColumn id="6" name="Muy alto .8" dataDxfId="13"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium11" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Tabla2" displayName="Tabla2" ref="A1:D13" totalsRowShown="0" headerRowDxfId="16" dataDxfId="15">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Tabla2" displayName="Tabla2" ref="A1:D13" totalsRowShown="0" headerRowDxfId="12" dataDxfId="11">
   <autoFilter ref="A1:D13"/>
   <tableColumns count="4">
-    <tableColumn id="1" name="Riesgo" dataDxfId="20"/>
-    <tableColumn id="2" name="Probabilidad de ocurrencia" dataDxfId="19"/>
-    <tableColumn id="3" name="Impacto" dataDxfId="18"/>
-    <tableColumn id="4" name="Estratégia de atención" dataDxfId="17"/>
+    <tableColumn id="1" name="Riesgo" dataDxfId="10"/>
+    <tableColumn id="2" name="Probabilidad de ocurrencia" dataDxfId="9"/>
+    <tableColumn id="3" name="Impacto" dataDxfId="8"/>
+    <tableColumn id="4" name="Estratégia de atención" dataDxfId="7"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium11" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Tabla3" displayName="Tabla3" ref="A1:E15" totalsRowShown="0" headerRowDxfId="1" dataDxfId="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Tabla3" displayName="Tabla3" ref="A1:E15" totalsRowShown="0" headerRowDxfId="6" dataDxfId="5">
   <autoFilter ref="A1:E15"/>
   <sortState ref="A2:E15">
-    <sortCondition ref="C1:C15"/>
+    <sortCondition ref="A1:A15"/>
   </sortState>
   <tableColumns count="5">
-    <tableColumn id="1" name="Actividad / Recurso" dataDxfId="6"/>
-    <tableColumn id="2" name="Ricardo" dataDxfId="5"/>
-    <tableColumn id="3" name="Mares" dataDxfId="4"/>
-    <tableColumn id="4" name="Andrés" dataDxfId="3"/>
-    <tableColumn id="5" name="Fernando" dataDxfId="2"/>
+    <tableColumn id="1" name="Actividad / Recurso" dataDxfId="4"/>
+    <tableColumn id="2" name="Ricardo" dataDxfId="3"/>
+    <tableColumn id="3" name="Mares" dataDxfId="2"/>
+    <tableColumn id="4" name="Andrés" dataDxfId="1"/>
+    <tableColumn id="5" name="Fernando" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium25" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1132,7 +1132,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H41"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
@@ -1145,243 +1145,243 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A1" s="14" t="s">
+      <c r="A1" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="14" t="s">
+      <c r="B1" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="C1" s="14" t="s">
+      <c r="C1" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="D1" s="14" t="s">
+      <c r="D1" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="E1" s="14" t="s">
+      <c r="E1" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="F1" s="14" t="s">
+      <c r="F1" s="12" t="s">
         <v>14</v>
       </c>
       <c r="G1" s="3"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" s="13" t="s">
+      <c r="A2" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="B2" s="16"/>
-      <c r="C2" s="16"/>
-      <c r="D2" s="14"/>
-      <c r="E2" s="14">
+      <c r="B2" s="14"/>
+      <c r="C2" s="14"/>
+      <c r="D2" s="12"/>
+      <c r="E2" s="12">
         <v>1</v>
       </c>
-      <c r="F2" s="16"/>
+      <c r="F2" s="14"/>
       <c r="G2" s="3"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" s="13" t="s">
+      <c r="A3" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="B3" s="16"/>
-      <c r="C3" s="16"/>
-      <c r="D3" s="16"/>
-      <c r="E3" s="16"/>
-      <c r="F3" s="14">
+      <c r="B3" s="14"/>
+      <c r="C3" s="14"/>
+      <c r="D3" s="14"/>
+      <c r="E3" s="14"/>
+      <c r="F3" s="12">
         <v>1</v>
       </c>
       <c r="G3" s="3"/>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" s="13" t="s">
+      <c r="A4" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="B4" s="16"/>
-      <c r="C4" s="16"/>
-      <c r="D4" s="14">
+      <c r="B4" s="14"/>
+      <c r="C4" s="14"/>
+      <c r="D4" s="12">
         <v>1</v>
       </c>
-      <c r="E4" s="16"/>
-      <c r="F4" s="16"/>
+      <c r="E4" s="14"/>
+      <c r="F4" s="14"/>
       <c r="G4" s="3"/>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" s="13" t="s">
+      <c r="A5" s="11" t="s">
         <v>31</v>
       </c>
-      <c r="B5" s="16"/>
-      <c r="C5" s="16"/>
-      <c r="D5" s="14"/>
-      <c r="E5" s="14">
+      <c r="B5" s="14"/>
+      <c r="C5" s="14"/>
+      <c r="D5" s="12"/>
+      <c r="E5" s="12">
         <v>1</v>
       </c>
-      <c r="F5" s="16"/>
+      <c r="F5" s="14"/>
       <c r="G5" s="3"/>
       <c r="H5" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" s="13" t="s">
+      <c r="A6" s="11" t="s">
         <v>34</v>
       </c>
-      <c r="B6" s="16"/>
-      <c r="C6" s="14">
+      <c r="B6" s="14"/>
+      <c r="C6" s="12">
         <v>1</v>
       </c>
-      <c r="D6" s="14"/>
-      <c r="E6" s="14"/>
-      <c r="F6" s="16"/>
+      <c r="D6" s="12"/>
+      <c r="E6" s="12"/>
+      <c r="F6" s="14"/>
       <c r="G6" s="3"/>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" s="13" t="s">
+      <c r="A7" s="11" t="s">
         <v>40</v>
       </c>
-      <c r="B7" s="16"/>
-      <c r="C7" s="14">
+      <c r="B7" s="14"/>
+      <c r="C7" s="12">
         <v>1</v>
       </c>
-      <c r="D7" s="16"/>
-      <c r="E7" s="16"/>
-      <c r="F7" s="16"/>
+      <c r="D7" s="14"/>
+      <c r="E7" s="14"/>
+      <c r="F7" s="14"/>
       <c r="G7" s="3"/>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8" s="13" t="s">
+      <c r="A8" s="11" t="s">
         <v>44</v>
       </c>
-      <c r="B8" s="14"/>
-      <c r="C8" s="14">
+      <c r="B8" s="12"/>
+      <c r="C8" s="12">
         <v>1</v>
       </c>
-      <c r="D8" s="14"/>
-      <c r="E8" s="14"/>
-      <c r="F8" s="14"/>
+      <c r="D8" s="12"/>
+      <c r="E8" s="12"/>
+      <c r="F8" s="12"/>
       <c r="G8" s="3"/>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9" s="13" t="s">
+      <c r="A9" s="11" t="s">
         <v>49</v>
       </c>
-      <c r="B9" s="16"/>
-      <c r="C9" s="16"/>
-      <c r="D9" s="14"/>
-      <c r="E9" s="14">
+      <c r="B9" s="14"/>
+      <c r="C9" s="14"/>
+      <c r="D9" s="12"/>
+      <c r="E9" s="12">
         <v>1</v>
       </c>
-      <c r="F9" s="16"/>
+      <c r="F9" s="14"/>
       <c r="G9" s="3"/>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A10" s="13" t="s">
+      <c r="A10" s="11" t="s">
         <v>54</v>
       </c>
-      <c r="B10" s="16"/>
-      <c r="C10" s="16"/>
-      <c r="D10" s="14">
+      <c r="B10" s="14"/>
+      <c r="C10" s="14"/>
+      <c r="D10" s="12">
         <v>1</v>
       </c>
-      <c r="E10" s="16"/>
-      <c r="F10" s="16"/>
+      <c r="E10" s="14"/>
+      <c r="F10" s="14"/>
       <c r="G10" s="3"/>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A11" s="13" t="s">
+      <c r="A11" s="11" t="s">
         <v>56</v>
       </c>
-      <c r="B11" s="14">
+      <c r="B11" s="12">
         <v>1</v>
       </c>
-      <c r="C11" s="16"/>
-      <c r="D11" s="16"/>
-      <c r="E11" s="16"/>
-      <c r="F11" s="16"/>
+      <c r="C11" s="14"/>
+      <c r="D11" s="14"/>
+      <c r="E11" s="14"/>
+      <c r="F11" s="14"/>
       <c r="G11" s="3"/>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A12" s="13" t="s">
+      <c r="A12" s="11" t="s">
         <v>58</v>
       </c>
-      <c r="B12" s="14">
+      <c r="B12" s="12">
         <v>1</v>
       </c>
-      <c r="C12" s="16"/>
-      <c r="D12" s="14"/>
-      <c r="E12" s="16"/>
-      <c r="F12" s="16"/>
+      <c r="C12" s="14"/>
+      <c r="D12" s="12"/>
+      <c r="E12" s="14"/>
+      <c r="F12" s="14"/>
       <c r="G12" s="3"/>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A13" s="13" t="s">
+      <c r="A13" s="11" t="s">
         <v>59</v>
       </c>
-      <c r="B13" s="14">
+      <c r="B13" s="12">
         <v>1</v>
       </c>
-      <c r="C13" s="16"/>
-      <c r="D13" s="16"/>
-      <c r="E13" s="14"/>
-      <c r="F13" s="16"/>
+      <c r="C13" s="14"/>
+      <c r="D13" s="14"/>
+      <c r="E13" s="12"/>
+      <c r="F13" s="14"/>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A14" s="13" t="s">
+      <c r="A14" s="11" t="s">
         <v>60</v>
       </c>
-      <c r="B14" s="17"/>
-      <c r="C14" s="18"/>
-      <c r="D14" s="18">
+      <c r="B14" s="15"/>
+      <c r="C14" s="16"/>
+      <c r="D14" s="16">
         <v>1</v>
       </c>
-      <c r="E14" s="17"/>
-      <c r="F14" s="17"/>
+      <c r="E14" s="15"/>
+      <c r="F14" s="15"/>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A15" s="13" t="s">
+      <c r="A15" s="11" t="s">
         <v>61</v>
       </c>
-      <c r="B15" s="14"/>
-      <c r="C15" s="14"/>
-      <c r="D15" s="14">
+      <c r="B15" s="12"/>
+      <c r="C15" s="12"/>
+      <c r="D15" s="12">
         <v>1</v>
       </c>
-      <c r="E15" s="14"/>
-      <c r="F15" s="14"/>
+      <c r="E15" s="12"/>
+      <c r="F15" s="12"/>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A16" s="13" t="s">
+      <c r="A16" s="11" t="s">
         <v>62</v>
       </c>
-      <c r="B16" s="14"/>
-      <c r="C16" s="16"/>
-      <c r="D16" s="14">
+      <c r="B16" s="12"/>
+      <c r="C16" s="14"/>
+      <c r="D16" s="12">
         <v>1</v>
       </c>
-      <c r="E16" s="16"/>
-      <c r="F16" s="16"/>
+      <c r="E16" s="14"/>
+      <c r="F16" s="14"/>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A17" s="13" t="s">
+      <c r="A17" s="11" t="s">
         <v>63</v>
       </c>
-      <c r="B17" s="14"/>
-      <c r="C17" s="16"/>
-      <c r="D17" s="16"/>
-      <c r="E17" s="14">
+      <c r="B17" s="12"/>
+      <c r="C17" s="14"/>
+      <c r="D17" s="14"/>
+      <c r="E17" s="12">
         <v>1</v>
       </c>
-      <c r="F17" s="16"/>
+      <c r="F17" s="14"/>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A18" s="13" t="s">
+      <c r="A18" s="11" t="s">
         <v>64</v>
       </c>
-      <c r="B18" s="16"/>
-      <c r="C18" s="16"/>
-      <c r="D18" s="16"/>
-      <c r="E18" s="14">
+      <c r="B18" s="14"/>
+      <c r="C18" s="14"/>
+      <c r="D18" s="14"/>
+      <c r="E18" s="12">
         <v>1</v>
       </c>
-      <c r="F18" s="16"/>
+      <c r="F18" s="14"/>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B19" s="2"/>
@@ -1591,184 +1591,184 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A1" s="13" t="s">
+      <c r="A1" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="13" t="s">
+      <c r="B1" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="C1" s="13" t="s">
+      <c r="C1" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="D1" s="13" t="s">
+      <c r="D1" s="11" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A2" s="14" t="s">
+      <c r="A2" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="B2" s="14">
+      <c r="B2" s="12">
         <v>0.5</v>
       </c>
-      <c r="C2" s="15">
+      <c r="C2" s="13">
         <v>0.75</v>
       </c>
-      <c r="D2" s="14" t="s">
+      <c r="D2" s="12" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A3" s="14" t="s">
+      <c r="A3" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="B3" s="14">
+      <c r="B3" s="12">
         <v>0.3</v>
       </c>
-      <c r="C3" s="15">
+      <c r="C3" s="13">
         <v>0.78</v>
       </c>
-      <c r="D3" s="14" t="s">
+      <c r="D3" s="12" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A4" s="14" t="s">
+      <c r="A4" s="12" t="s">
         <v>24</v>
       </c>
-      <c r="B4" s="14">
+      <c r="B4" s="12">
         <v>0.4</v>
       </c>
-      <c r="C4" s="15">
+      <c r="C4" s="13">
         <v>0.7</v>
       </c>
-      <c r="D4" s="14" t="s">
+      <c r="D4" s="12" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A5" s="14" t="s">
+      <c r="A5" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="B5" s="14">
+      <c r="B5" s="12">
         <v>0.05</v>
       </c>
-      <c r="C5" s="15">
+      <c r="C5" s="13">
         <v>0.4</v>
       </c>
-      <c r="D5" s="14" t="s">
+      <c r="D5" s="12" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A6" s="14" t="s">
+      <c r="A6" s="12" t="s">
         <v>29</v>
       </c>
-      <c r="B6" s="14">
+      <c r="B6" s="12">
         <v>0.3</v>
       </c>
-      <c r="C6" s="15">
+      <c r="C6" s="13">
         <v>0.8</v>
       </c>
-      <c r="D6" s="14" t="s">
+      <c r="D6" s="12" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A7" s="14" t="s">
+      <c r="A7" s="12" t="s">
         <v>32</v>
       </c>
-      <c r="B7" s="14">
+      <c r="B7" s="12">
         <v>0.4</v>
       </c>
-      <c r="C7" s="15">
+      <c r="C7" s="13">
         <v>0.65</v>
       </c>
-      <c r="D7" s="14" t="s">
+      <c r="D7" s="12" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A8" s="14" t="s">
+      <c r="A8" s="12" t="s">
         <v>35</v>
       </c>
-      <c r="B8" s="14">
+      <c r="B8" s="12">
         <v>0.6</v>
       </c>
-      <c r="C8" s="15">
+      <c r="C8" s="13">
         <v>0.6</v>
       </c>
-      <c r="D8" s="14" t="s">
+      <c r="D8" s="12" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A9" s="14" t="s">
+      <c r="A9" s="12" t="s">
         <v>37</v>
       </c>
-      <c r="B9" s="14">
+      <c r="B9" s="12">
         <v>0.3</v>
       </c>
-      <c r="C9" s="15">
+      <c r="C9" s="13">
         <v>0.5</v>
       </c>
-      <c r="D9" s="14" t="s">
+      <c r="D9" s="12" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A10" s="14" t="s">
+      <c r="A10" s="12" t="s">
         <v>39</v>
       </c>
-      <c r="B10" s="14">
+      <c r="B10" s="12">
         <v>0.6</v>
       </c>
-      <c r="C10" s="15">
+      <c r="C10" s="13">
         <v>0.75</v>
       </c>
-      <c r="D10" s="14" t="s">
+      <c r="D10" s="12" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A11" s="14" t="s">
+      <c r="A11" s="12" t="s">
         <v>43</v>
       </c>
-      <c r="B11" s="14">
+      <c r="B11" s="12">
         <v>0.8</v>
       </c>
-      <c r="C11" s="15">
+      <c r="C11" s="13">
         <v>0.7</v>
       </c>
-      <c r="D11" s="14" t="s">
+      <c r="D11" s="12" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A12" s="14" t="s">
+      <c r="A12" s="12" t="s">
         <v>48</v>
       </c>
-      <c r="B12" s="14">
+      <c r="B12" s="12">
         <v>0.3</v>
       </c>
-      <c r="C12" s="15">
+      <c r="C12" s="13">
         <v>0.8</v>
       </c>
-      <c r="D12" s="14" t="s">
+      <c r="D12" s="12" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="14" t="s">
+      <c r="A13" s="12" t="s">
         <v>52</v>
       </c>
-      <c r="B13" s="14">
+      <c r="B13" s="12">
         <v>0.9</v>
       </c>
-      <c r="C13" s="15">
+      <c r="C13" s="13">
         <v>0.8</v>
       </c>
-      <c r="D13" s="14" t="s">
+      <c r="D13" s="12" t="s">
         <v>66</v>
       </c>
     </row>
@@ -1785,8 +1785,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:E3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A13" sqref="A13:E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1796,19 +1796,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A1" s="12" t="s">
+      <c r="A1" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="12" t="s">
+      <c r="B1" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="C1" s="12" t="s">
+      <c r="C1" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="D1" s="12" t="s">
+      <c r="D1" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="E1" s="12" t="s">
+      <c r="E1" s="10" t="s">
         <v>9</v>
       </c>
       <c r="F1" s="2"/>
@@ -1816,42 +1816,42 @@
       <c r="H1" s="2"/>
     </row>
     <row r="2" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A2" s="11" t="s">
-        <v>31</v>
-      </c>
-      <c r="B2" s="12" t="s">
-        <v>17</v>
-      </c>
-      <c r="C2" s="12" t="s">
-        <v>46</v>
-      </c>
-      <c r="D2" s="12" t="s">
-        <v>17</v>
-      </c>
-      <c r="E2" s="12" t="s">
+      <c r="A2" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="B2" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="C2" s="10" t="s">
         <v>18</v>
       </c>
+      <c r="D2" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="E2" s="10" t="s">
+        <v>17</v>
+      </c>
       <c r="F2" s="2"/>
-      <c r="G2" s="9" t="s">
+      <c r="G2" s="17" t="s">
         <v>19</v>
       </c>
-      <c r="H2" s="10"/>
+      <c r="H2" s="18"/>
     </row>
     <row r="3" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A3" s="11" t="s">
-        <v>44</v>
-      </c>
-      <c r="B3" s="12" t="s">
+      <c r="A3" s="9" t="s">
+        <v>59</v>
+      </c>
+      <c r="B3" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="C3" s="12" t="s">
+      <c r="C3" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="D3" s="10" t="s">
         <v>51</v>
       </c>
-      <c r="D3" s="12" t="s">
-        <v>17</v>
-      </c>
-      <c r="E3" s="12" t="s">
-        <v>46</v>
+      <c r="E3" s="10" t="s">
+        <v>17</v>
       </c>
       <c r="F3" s="2"/>
       <c r="G3" s="4" t="s">
@@ -1862,19 +1862,19 @@
       </c>
     </row>
     <row r="4" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A4" s="11" t="s">
-        <v>63</v>
-      </c>
-      <c r="B4" s="12" t="s">
-        <v>51</v>
-      </c>
-      <c r="C4" s="12" t="s">
-        <v>51</v>
-      </c>
-      <c r="D4" s="12" t="s">
+      <c r="A4" s="9" t="s">
+        <v>62</v>
+      </c>
+      <c r="B4" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="C4" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="E4" s="12" t="s">
+      <c r="D4" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="E4" s="10" t="s">
         <v>51</v>
       </c>
       <c r="F4" s="2"/>
@@ -1886,19 +1886,19 @@
       </c>
     </row>
     <row r="5" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A5" s="11" t="s">
+      <c r="A5" s="9" t="s">
         <v>40</v>
       </c>
-      <c r="B5" s="12" t="s">
-        <v>17</v>
-      </c>
-      <c r="C5" s="12" t="s">
+      <c r="B5" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="C5" s="10" t="s">
         <v>51</v>
       </c>
-      <c r="D5" s="12" t="s">
+      <c r="D5" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="E5" s="12" t="s">
+      <c r="E5" s="10" t="s">
         <v>17</v>
       </c>
       <c r="F5" s="2"/>
@@ -1913,20 +1913,20 @@
       </c>
     </row>
     <row r="6" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A6" s="11" t="s">
-        <v>59</v>
-      </c>
-      <c r="B6" s="12" t="s">
+      <c r="A6" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="B6" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="C6" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="D6" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="E6" s="10" t="s">
         <v>18</v>
-      </c>
-      <c r="C6" s="12" t="s">
-        <v>17</v>
-      </c>
-      <c r="D6" s="12" t="s">
-        <v>51</v>
-      </c>
-      <c r="E6" s="12" t="s">
-        <v>17</v>
       </c>
       <c r="F6" s="2"/>
       <c r="G6" s="4" t="s">
@@ -1937,59 +1937,59 @@
       </c>
     </row>
     <row r="7" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A7" s="11" t="s">
-        <v>16</v>
-      </c>
-      <c r="B7" s="12" t="s">
-        <v>17</v>
-      </c>
-      <c r="C7" s="12" t="s">
-        <v>17</v>
-      </c>
-      <c r="D7" s="12" t="s">
-        <v>17</v>
-      </c>
-      <c r="E7" s="12" t="s">
+      <c r="A7" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="B7" s="10" t="s">
         <v>18</v>
+      </c>
+      <c r="C7" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="D7" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="E7" s="10" t="s">
+        <v>46</v>
       </c>
       <c r="F7" s="2"/>
       <c r="G7" s="2"/>
       <c r="H7" s="2"/>
     </row>
     <row r="8" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A8" s="11" t="s">
-        <v>54</v>
-      </c>
-      <c r="B8" s="12" t="s">
-        <v>17</v>
-      </c>
-      <c r="C8" s="12" t="s">
-        <v>17</v>
-      </c>
-      <c r="D8" s="12" t="s">
-        <v>17</v>
-      </c>
-      <c r="E8" s="12" t="s">
+      <c r="A8" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="B8" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="C8" s="10" t="s">
         <v>18</v>
+      </c>
+      <c r="D8" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="E8" s="10" t="s">
+        <v>17</v>
       </c>
       <c r="F8" s="2"/>
       <c r="G8" s="2"/>
       <c r="H8" s="2"/>
     </row>
     <row r="9" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A9" s="11" t="s">
-        <v>62</v>
-      </c>
-      <c r="B9" s="12" t="s">
-        <v>17</v>
-      </c>
-      <c r="C9" s="12" t="s">
+      <c r="A9" s="9" t="s">
+        <v>58</v>
+      </c>
+      <c r="B9" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="C9" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="D9" s="12" t="s">
-        <v>17</v>
-      </c>
-      <c r="E9" s="12" t="s">
+      <c r="D9" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="E9" s="10" t="s">
         <v>51</v>
       </c>
       <c r="F9" s="2"/>
@@ -1997,79 +1997,79 @@
       <c r="H9" s="2"/>
     </row>
     <row r="10" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A10" s="11" t="s">
-        <v>58</v>
-      </c>
-      <c r="B10" s="12" t="s">
-        <v>17</v>
-      </c>
-      <c r="C10" s="12" t="s">
+      <c r="A10" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="B10" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="D10" s="12" t="s">
-        <v>17</v>
-      </c>
-      <c r="E10" s="12" t="s">
-        <v>51</v>
+      <c r="C10" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="D10" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="E10" s="10" t="s">
+        <v>18</v>
       </c>
       <c r="F10" s="2"/>
       <c r="G10" s="2"/>
       <c r="H10" s="2"/>
     </row>
     <row r="11" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A11" s="11" t="s">
-        <v>23</v>
-      </c>
-      <c r="B11" s="12" t="s">
-        <v>17</v>
-      </c>
-      <c r="C11" s="12" t="s">
+      <c r="A11" s="9" t="s">
+        <v>60</v>
+      </c>
+      <c r="B11" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="D11" s="12" t="s">
-        <v>17</v>
-      </c>
-      <c r="E11" s="12" t="s">
-        <v>17</v>
+      <c r="C11" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="D11" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="E11" s="10" t="s">
+        <v>18</v>
       </c>
       <c r="F11" s="2"/>
       <c r="G11" s="2"/>
       <c r="H11" s="2"/>
     </row>
     <row r="12" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A12" s="11" t="s">
-        <v>34</v>
-      </c>
-      <c r="B12" s="12" t="s">
-        <v>17</v>
-      </c>
-      <c r="C12" s="12" t="s">
+      <c r="A12" s="9" t="s">
+        <v>63</v>
+      </c>
+      <c r="B12" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="C12" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="D12" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="D12" s="12" t="s">
-        <v>17</v>
-      </c>
-      <c r="E12" s="12" t="s">
-        <v>17</v>
+      <c r="E12" s="10" t="s">
+        <v>51</v>
       </c>
       <c r="F12" s="2"/>
       <c r="G12" s="2"/>
       <c r="H12" s="2"/>
     </row>
     <row r="13" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A13" s="11" t="s">
-        <v>49</v>
-      </c>
-      <c r="B13" s="12" t="s">
+      <c r="A13" s="9" t="s">
+        <v>61</v>
+      </c>
+      <c r="B13" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="C13" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="C13" s="12" t="s">
-        <v>18</v>
-      </c>
-      <c r="D13" s="12" t="s">
-        <v>18</v>
-      </c>
-      <c r="E13" s="12" t="s">
+      <c r="D13" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="E13" s="10" t="s">
         <v>18</v>
       </c>
       <c r="F13" s="2"/>
@@ -2077,19 +2077,19 @@
       <c r="H13" s="2"/>
     </row>
     <row r="14" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A14" s="11" t="s">
-        <v>60</v>
-      </c>
-      <c r="B14" s="12" t="s">
-        <v>18</v>
-      </c>
-      <c r="C14" s="12" t="s">
-        <v>18</v>
-      </c>
-      <c r="D14" s="12" t="s">
-        <v>18</v>
-      </c>
-      <c r="E14" s="12" t="s">
+      <c r="A14" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="B14" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="C14" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="D14" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="E14" s="10" t="s">
         <v>18</v>
       </c>
       <c r="F14" s="2"/>
@@ -2097,19 +2097,19 @@
       <c r="H14" s="2"/>
     </row>
     <row r="15" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A15" s="11" t="s">
-        <v>61</v>
-      </c>
-      <c r="B15" s="12" t="s">
-        <v>51</v>
-      </c>
-      <c r="C15" s="12" t="s">
-        <v>18</v>
-      </c>
-      <c r="D15" s="12" t="s">
-        <v>51</v>
-      </c>
-      <c r="E15" s="12" t="s">
+      <c r="A15" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="B15" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="C15" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="D15" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="E15" s="10" t="s">
         <v>18</v>
       </c>
       <c r="F15" s="2"/>

</xml_diff>

<commit_message>
Creo la lista de entregables faltan los puntos 3 6 9
</commit_message>
<xml_diff>
--- a/riesgos.xlsx
+++ b/riesgos.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Impactos" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="74">
   <si>
     <t>Actividad / Recurso</t>
   </si>
@@ -222,6 +222,27 @@
   </si>
   <si>
     <t>Reajustar el Proyecto</t>
+  </si>
+  <si>
+    <t>Se presento el problema</t>
+  </si>
+  <si>
+    <t>Si</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>Resumen detallado</t>
+  </si>
+  <si>
+    <t xml:space="preserve">En conclusión tener un plan de riesgos ayuda a mantener la estabilidad en un proyecto por medio de la erradicación o mitigación de los mismo de este modo aprendimos que los riesgos pueden ir desde los más catastroficos hasta los más banales como que una computadora deje de funcionar, y al ir generando experiencia, te da ideas de los riesgos más comunes en la administración de proyectos y como hay formas de mitigar o erradicar esos problemas </t>
+  </si>
+  <si>
+    <t>Dispositivo no funcional</t>
+  </si>
+  <si>
+    <t>Reacomodar tareas o rentar dispositivo para horas de trabajo</t>
   </si>
 </sst>
 </file>
@@ -335,7 +356,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -349,17 +370,180 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="9" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="21">
+  <dxfs count="22">
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Raleway"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor rgb="FFD9D9D9"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Raleway"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor rgb="FFD9D9D9"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Raleway"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="13" formatCode="0%"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Raleway"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="13" formatCode="0%"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor rgb="FFD9D9D9"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Raleway"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor rgb="FFD9D9D9"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Raleway"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor rgb="FFD9D9D9"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -517,127 +701,6 @@
       </font>
       <fill>
         <patternFill patternType="none">
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color auto="1"/>
-        <name val="Raleway"/>
-        <scheme val="none"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor rgb="FFD9D9D9"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color auto="1"/>
-        <name val="Raleway"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="13" formatCode="0%"/>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor rgb="FFD9D9D9"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color auto="1"/>
-        <name val="Raleway"/>
-        <scheme val="none"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor rgb="FFD9D9D9"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color auto="1"/>
-        <name val="Raleway"/>
-        <scheme val="none"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor rgb="FFD9D9D9"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color auto="1"/>
-        <name val="Raleway"/>
-        <scheme val="none"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor rgb="FFD9D9D9"/>
           <bgColor auto="1"/>
         </patternFill>
       </fill>
@@ -823,45 +886,46 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabla1" displayName="Tabla1" ref="A1:F18" totalsRowShown="0" headerRowDxfId="20" dataDxfId="19">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabla1" displayName="Tabla1" ref="A1:F18" totalsRowShown="0" headerRowDxfId="21" dataDxfId="20">
   <autoFilter ref="A1:F18"/>
   <tableColumns count="6">
-    <tableColumn id="1" name="Objetivos del proyecto" dataDxfId="18"/>
-    <tableColumn id="2" name="Muy bajo .05" dataDxfId="17"/>
-    <tableColumn id="3" name="Bajo .1" dataDxfId="16"/>
-    <tableColumn id="4" name="Moderado .2" dataDxfId="15"/>
-    <tableColumn id="5" name="Alto .4" dataDxfId="14"/>
-    <tableColumn id="6" name="Muy alto .8" dataDxfId="13"/>
+    <tableColumn id="1" name="Objetivos del proyecto" dataDxfId="19"/>
+    <tableColumn id="2" name="Muy bajo .05" dataDxfId="18"/>
+    <tableColumn id="3" name="Bajo .1" dataDxfId="17"/>
+    <tableColumn id="4" name="Moderado .2" dataDxfId="16"/>
+    <tableColumn id="5" name="Alto .4" dataDxfId="15"/>
+    <tableColumn id="6" name="Muy alto .8" dataDxfId="14"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium11" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Tabla2" displayName="Tabla2" ref="A1:D13" totalsRowShown="0" headerRowDxfId="12" dataDxfId="11">
-  <autoFilter ref="A1:D13"/>
-  <tableColumns count="4">
-    <tableColumn id="1" name="Riesgo" dataDxfId="10"/>
-    <tableColumn id="2" name="Probabilidad de ocurrencia" dataDxfId="9"/>
-    <tableColumn id="3" name="Impacto" dataDxfId="8"/>
-    <tableColumn id="4" name="Estratégia de atención" dataDxfId="7"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Tabla2" displayName="Tabla2" ref="A1:E13" totalsRowShown="0" headerRowDxfId="13" dataDxfId="0">
+  <autoFilter ref="A1:E13"/>
+  <tableColumns count="5">
+    <tableColumn id="1" name="Riesgo" dataDxfId="5"/>
+    <tableColumn id="2" name="Probabilidad de ocurrencia" dataDxfId="4"/>
+    <tableColumn id="3" name="Impacto" dataDxfId="3"/>
+    <tableColumn id="5" name="Se presento el problema" dataDxfId="2"/>
+    <tableColumn id="4" name="Estratégia de atención" dataDxfId="1"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium11" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Tabla3" displayName="Tabla3" ref="A1:E15" totalsRowShown="0" headerRowDxfId="6" dataDxfId="5">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Tabla3" displayName="Tabla3" ref="A1:E15" totalsRowShown="0" headerRowDxfId="12" dataDxfId="11">
   <autoFilter ref="A1:E15"/>
   <sortState ref="A2:E15">
     <sortCondition ref="A1:A15"/>
   </sortState>
   <tableColumns count="5">
-    <tableColumn id="1" name="Actividad / Recurso" dataDxfId="4"/>
-    <tableColumn id="2" name="Ricardo" dataDxfId="3"/>
-    <tableColumn id="3" name="Mares" dataDxfId="2"/>
-    <tableColumn id="4" name="Andrés" dataDxfId="1"/>
-    <tableColumn id="5" name="Fernando" dataDxfId="0"/>
+    <tableColumn id="1" name="Actividad / Recurso" dataDxfId="10"/>
+    <tableColumn id="2" name="Ricardo" dataDxfId="9"/>
+    <tableColumn id="3" name="Mares" dataDxfId="8"/>
+    <tableColumn id="4" name="Andrés" dataDxfId="7"/>
+    <tableColumn id="5" name="Fernando" dataDxfId="6"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium25" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1169,23 +1233,23 @@
       <c r="A2" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="B2" s="14"/>
-      <c r="C2" s="14"/>
+      <c r="B2" s="13"/>
+      <c r="C2" s="13"/>
       <c r="D2" s="12"/>
       <c r="E2" s="12">
         <v>1</v>
       </c>
-      <c r="F2" s="14"/>
+      <c r="F2" s="13"/>
       <c r="G2" s="3"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="B3" s="14"/>
-      <c r="C3" s="14"/>
-      <c r="D3" s="14"/>
-      <c r="E3" s="14"/>
+      <c r="B3" s="13"/>
+      <c r="C3" s="13"/>
+      <c r="D3" s="13"/>
+      <c r="E3" s="13"/>
       <c r="F3" s="12">
         <v>1</v>
       </c>
@@ -1195,26 +1259,26 @@
       <c r="A4" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="B4" s="14"/>
-      <c r="C4" s="14"/>
+      <c r="B4" s="13"/>
+      <c r="C4" s="13"/>
       <c r="D4" s="12">
         <v>1</v>
       </c>
-      <c r="E4" s="14"/>
-      <c r="F4" s="14"/>
+      <c r="E4" s="13"/>
+      <c r="F4" s="13"/>
       <c r="G4" s="3"/>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="11" t="s">
         <v>31</v>
       </c>
-      <c r="B5" s="14"/>
-      <c r="C5" s="14"/>
+      <c r="B5" s="13"/>
+      <c r="C5" s="13"/>
       <c r="D5" s="12"/>
       <c r="E5" s="12">
         <v>1</v>
       </c>
-      <c r="F5" s="14"/>
+      <c r="F5" s="13"/>
       <c r="G5" s="3"/>
       <c r="H5" t="s">
         <v>65</v>
@@ -1224,26 +1288,26 @@
       <c r="A6" s="11" t="s">
         <v>34</v>
       </c>
-      <c r="B6" s="14"/>
+      <c r="B6" s="13"/>
       <c r="C6" s="12">
         <v>1</v>
       </c>
       <c r="D6" s="12"/>
       <c r="E6" s="12"/>
-      <c r="F6" s="14"/>
+      <c r="F6" s="13"/>
       <c r="G6" s="3"/>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="11" t="s">
         <v>40</v>
       </c>
-      <c r="B7" s="14"/>
+      <c r="B7" s="13"/>
       <c r="C7" s="12">
         <v>1</v>
       </c>
-      <c r="D7" s="14"/>
-      <c r="E7" s="14"/>
-      <c r="F7" s="14"/>
+      <c r="D7" s="13"/>
+      <c r="E7" s="13"/>
+      <c r="F7" s="13"/>
       <c r="G7" s="3"/>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
@@ -1263,26 +1327,26 @@
       <c r="A9" s="11" t="s">
         <v>49</v>
       </c>
-      <c r="B9" s="14"/>
-      <c r="C9" s="14"/>
+      <c r="B9" s="13"/>
+      <c r="C9" s="13"/>
       <c r="D9" s="12"/>
       <c r="E9" s="12">
         <v>1</v>
       </c>
-      <c r="F9" s="14"/>
+      <c r="F9" s="13"/>
       <c r="G9" s="3"/>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="11" t="s">
         <v>54</v>
       </c>
-      <c r="B10" s="14"/>
-      <c r="C10" s="14"/>
+      <c r="B10" s="13"/>
+      <c r="C10" s="13"/>
       <c r="D10" s="12">
         <v>1</v>
       </c>
-      <c r="E10" s="14"/>
-      <c r="F10" s="14"/>
+      <c r="E10" s="13"/>
+      <c r="F10" s="13"/>
       <c r="G10" s="3"/>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
@@ -1292,10 +1356,10 @@
       <c r="B11" s="12">
         <v>1</v>
       </c>
-      <c r="C11" s="14"/>
-      <c r="D11" s="14"/>
-      <c r="E11" s="14"/>
-      <c r="F11" s="14"/>
+      <c r="C11" s="13"/>
+      <c r="D11" s="13"/>
+      <c r="E11" s="13"/>
+      <c r="F11" s="13"/>
       <c r="G11" s="3"/>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
@@ -1305,10 +1369,10 @@
       <c r="B12" s="12">
         <v>1</v>
       </c>
-      <c r="C12" s="14"/>
+      <c r="C12" s="13"/>
       <c r="D12" s="12"/>
-      <c r="E12" s="14"/>
-      <c r="F12" s="14"/>
+      <c r="E12" s="13"/>
+      <c r="F12" s="13"/>
       <c r="G12" s="3"/>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
@@ -1318,22 +1382,22 @@
       <c r="B13" s="12">
         <v>1</v>
       </c>
-      <c r="C13" s="14"/>
-      <c r="D13" s="14"/>
+      <c r="C13" s="13"/>
+      <c r="D13" s="13"/>
       <c r="E13" s="12"/>
-      <c r="F13" s="14"/>
+      <c r="F13" s="13"/>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="11" t="s">
         <v>60</v>
       </c>
-      <c r="B14" s="15"/>
-      <c r="C14" s="16"/>
-      <c r="D14" s="16">
+      <c r="B14" s="14"/>
+      <c r="C14" s="15"/>
+      <c r="D14" s="15">
         <v>1</v>
       </c>
-      <c r="E14" s="15"/>
-      <c r="F14" s="15"/>
+      <c r="E14" s="14"/>
+      <c r="F14" s="14"/>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="11" t="s">
@@ -1352,36 +1416,36 @@
         <v>62</v>
       </c>
       <c r="B16" s="12"/>
-      <c r="C16" s="14"/>
+      <c r="C16" s="13"/>
       <c r="D16" s="12">
         <v>1</v>
       </c>
-      <c r="E16" s="14"/>
-      <c r="F16" s="14"/>
+      <c r="E16" s="13"/>
+      <c r="F16" s="13"/>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="11" t="s">
         <v>63</v>
       </c>
       <c r="B17" s="12"/>
-      <c r="C17" s="14"/>
-      <c r="D17" s="14"/>
+      <c r="C17" s="13"/>
+      <c r="D17" s="13"/>
       <c r="E17" s="12">
         <v>1</v>
       </c>
-      <c r="F17" s="14"/>
+      <c r="F17" s="13"/>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="11" t="s">
         <v>64</v>
       </c>
-      <c r="B18" s="14"/>
-      <c r="C18" s="14"/>
-      <c r="D18" s="14"/>
+      <c r="B18" s="13"/>
+      <c r="C18" s="13"/>
+      <c r="D18" s="13"/>
       <c r="E18" s="12">
         <v>1</v>
       </c>
-      <c r="F18" s="14"/>
+      <c r="F18" s="13"/>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B19" s="2"/>
@@ -1576,205 +1640,304 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D13"/>
+  <dimension ref="A1:E19"/>
   <sheetViews>
-    <sheetView topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="A23" sqref="A23:A24"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="51" customWidth="1"/>
-    <col min="2" max="2" width="29.42578125" customWidth="1"/>
-    <col min="3" max="3" width="17.140625" customWidth="1"/>
-    <col min="4" max="4" width="62" customWidth="1"/>
+    <col min="1" max="1" width="34.42578125" customWidth="1"/>
+    <col min="2" max="2" width="19.5703125" customWidth="1"/>
+    <col min="3" max="4" width="17.140625" customWidth="1"/>
+    <col min="5" max="5" width="63.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A1" s="11" t="s">
+    <row r="1" spans="1:5" ht="31.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="18" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="11" t="s">
+      <c r="B1" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="C1" s="11" t="s">
+      <c r="C1" s="18" t="s">
         <v>8</v>
       </c>
-      <c r="D1" s="11" t="s">
+      <c r="D1" s="19" t="s">
+        <v>67</v>
+      </c>
+      <c r="E1" s="18" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A2" s="12" t="s">
+    <row r="2" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="22" t="s">
         <v>15</v>
       </c>
-      <c r="B2" s="12">
+      <c r="B2" s="22">
         <v>0.5</v>
       </c>
-      <c r="C2" s="13">
+      <c r="C2" s="23">
         <v>0.75</v>
       </c>
-      <c r="D2" s="12" t="s">
+      <c r="D2" s="23" t="s">
+        <v>68</v>
+      </c>
+      <c r="E2" s="22" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A3" s="12" t="s">
+    <row r="3" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="22" t="s">
         <v>21</v>
       </c>
-      <c r="B3" s="12">
+      <c r="B3" s="22">
         <v>0.3</v>
       </c>
-      <c r="C3" s="13">
+      <c r="C3" s="23">
         <v>0.78</v>
       </c>
-      <c r="D3" s="12" t="s">
+      <c r="D3" s="23" t="s">
+        <v>69</v>
+      </c>
+      <c r="E3" s="22" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A4" s="12" t="s">
+    <row r="4" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="22" t="s">
         <v>24</v>
       </c>
-      <c r="B4" s="12">
+      <c r="B4" s="22">
         <v>0.4</v>
       </c>
-      <c r="C4" s="13">
+      <c r="C4" s="23">
         <v>0.7</v>
       </c>
-      <c r="D4" s="12" t="s">
+      <c r="D4" s="23" t="s">
+        <v>69</v>
+      </c>
+      <c r="E4" s="22" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A5" s="12" t="s">
+    <row r="5" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="22" t="s">
         <v>26</v>
       </c>
-      <c r="B5" s="12">
+      <c r="B5" s="22">
         <v>0.05</v>
       </c>
-      <c r="C5" s="13">
+      <c r="C5" s="23">
         <v>0.4</v>
       </c>
-      <c r="D5" s="12" t="s">
+      <c r="D5" s="23" t="s">
+        <v>69</v>
+      </c>
+      <c r="E5" s="22" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A6" s="12" t="s">
+    <row r="6" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="22" t="s">
         <v>29</v>
       </c>
-      <c r="B6" s="12">
+      <c r="B6" s="22">
         <v>0.3</v>
       </c>
-      <c r="C6" s="13">
+      <c r="C6" s="23">
         <v>0.8</v>
       </c>
-      <c r="D6" s="12" t="s">
+      <c r="D6" s="23" t="s">
+        <v>69</v>
+      </c>
+      <c r="E6" s="22" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A7" s="12" t="s">
+    <row r="7" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="22" t="s">
         <v>32</v>
       </c>
-      <c r="B7" s="12">
+      <c r="B7" s="22">
         <v>0.4</v>
       </c>
-      <c r="C7" s="13">
+      <c r="C7" s="23">
         <v>0.65</v>
       </c>
-      <c r="D7" s="12" t="s">
+      <c r="D7" s="23" t="s">
+        <v>69</v>
+      </c>
+      <c r="E7" s="22" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A8" s="12" t="s">
+    <row r="8" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="22" t="s">
         <v>35</v>
       </c>
-      <c r="B8" s="12">
+      <c r="B8" s="22">
         <v>0.6</v>
       </c>
-      <c r="C8" s="13">
+      <c r="C8" s="23">
         <v>0.6</v>
       </c>
-      <c r="D8" s="12" t="s">
+      <c r="D8" s="23" t="s">
+        <v>68</v>
+      </c>
+      <c r="E8" s="22" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A9" s="12" t="s">
+    <row r="9" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="22" t="s">
         <v>37</v>
       </c>
-      <c r="B9" s="12">
+      <c r="B9" s="22">
         <v>0.3</v>
       </c>
-      <c r="C9" s="13">
+      <c r="C9" s="23">
         <v>0.5</v>
       </c>
-      <c r="D9" s="12" t="s">
+      <c r="D9" s="23" t="s">
+        <v>69</v>
+      </c>
+      <c r="E9" s="22" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A10" s="12" t="s">
+    <row r="10" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="22" t="s">
         <v>39</v>
       </c>
-      <c r="B10" s="12">
+      <c r="B10" s="22">
         <v>0.6</v>
       </c>
-      <c r="C10" s="13">
+      <c r="C10" s="23">
         <v>0.75</v>
       </c>
-      <c r="D10" s="12" t="s">
+      <c r="D10" s="23" t="s">
+        <v>69</v>
+      </c>
+      <c r="E10" s="22" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A11" s="12" t="s">
+    <row r="11" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="22" t="s">
         <v>43</v>
       </c>
-      <c r="B11" s="12">
+      <c r="B11" s="22">
         <v>0.8</v>
       </c>
-      <c r="C11" s="13">
+      <c r="C11" s="23">
         <v>0.7</v>
       </c>
-      <c r="D11" s="12" t="s">
+      <c r="D11" s="23" t="s">
+        <v>69</v>
+      </c>
+      <c r="E11" s="22" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="12" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A12" s="12" t="s">
+    <row r="12" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="22" t="s">
         <v>48</v>
       </c>
-      <c r="B12" s="12">
+      <c r="B12" s="22">
         <v>0.3</v>
       </c>
-      <c r="C12" s="13">
+      <c r="C12" s="23">
         <v>0.8</v>
       </c>
-      <c r="D12" s="12" t="s">
+      <c r="D12" s="23" t="s">
+        <v>69</v>
+      </c>
+      <c r="E12" s="22" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="13" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="12" t="s">
+    <row r="13" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="22" t="s">
         <v>52</v>
       </c>
-      <c r="B13" s="12">
+      <c r="B13" s="22">
         <v>0.9</v>
       </c>
-      <c r="C13" s="13">
+      <c r="C13" s="23">
         <v>0.8</v>
       </c>
-      <c r="D13" s="12" t="s">
+      <c r="D13" s="23" t="s">
+        <v>68</v>
+      </c>
+      <c r="E13" s="22" t="s">
         <v>66</v>
       </c>
     </row>
+    <row r="14" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="22" t="s">
+        <v>72</v>
+      </c>
+      <c r="B14" s="22">
+        <v>0.9</v>
+      </c>
+      <c r="C14" s="23">
+        <v>0.75</v>
+      </c>
+      <c r="D14" s="23" t="s">
+        <v>68</v>
+      </c>
+      <c r="E14" s="22" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="20" t="s">
+        <v>70</v>
+      </c>
+      <c r="B15" s="20"/>
+      <c r="C15" s="20"/>
+      <c r="D15" s="20"/>
+      <c r="E15" s="20"/>
+    </row>
+    <row r="16" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A16" s="21" t="s">
+        <v>71</v>
+      </c>
+      <c r="B16" s="21"/>
+      <c r="C16" s="21"/>
+      <c r="D16" s="21"/>
+      <c r="E16" s="21"/>
+    </row>
+    <row r="17" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="21"/>
+      <c r="B17" s="21"/>
+      <c r="C17" s="21"/>
+      <c r="D17" s="21"/>
+      <c r="E17" s="21"/>
+    </row>
+    <row r="18" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A18" s="21"/>
+      <c r="B18" s="21"/>
+      <c r="C18" s="21"/>
+      <c r="D18" s="21"/>
+      <c r="E18" s="21"/>
+    </row>
+    <row r="19" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A19" s="21"/>
+      <c r="B19" s="21"/>
+      <c r="C19" s="21"/>
+      <c r="D19" s="21"/>
+      <c r="E19" s="21"/>
+    </row>
   </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A15:E15"/>
+    <mergeCell ref="A16:E19"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+  <pageSetup paperSize="5" orientation="landscape" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
   <tableParts count="1">
     <tablePart r:id="rId2"/>
   </tableParts>
@@ -1785,7 +1948,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A13" sqref="A13:E13"/>
     </sheetView>
   </sheetViews>
@@ -1832,10 +1995,10 @@
         <v>17</v>
       </c>
       <c r="F2" s="2"/>
-      <c r="G2" s="17" t="s">
+      <c r="G2" s="16" t="s">
         <v>19</v>
       </c>
-      <c r="H2" s="18"/>
+      <c r="H2" s="17"/>
     </row>
     <row r="3" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A3" s="9" t="s">
@@ -2121,8 +2284,9 @@
     <mergeCell ref="G2:H2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="5" orientation="landscape" r:id="rId1"/>
   <tableParts count="1">
-    <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>